<commit_message>
fix Leicester v Everton error
</commit_message>
<xml_diff>
--- a/Data/EPL_fixtures.xlsx
+++ b/Data/EPL_fixtures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.mark\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.mark\Downloads\EPL_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008CDA9C-D0EA-4B5D-A827-BB957BE6E3BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F389076-CDAA-42FD-A4C9-E326296E9B86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FB97F535-5B47-48FC-ABD3-A15F766655E8}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="All Fixtures" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Goals!$P$1:$P$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Goals!$A$1:$I$935</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Matches Played'!$B$1:$I$289</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44816EDD-419E-4C8B-9494-D47F59C094B5}">
   <dimension ref="A1:P935"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A899" workbookViewId="0">
+      <selection sqref="A1:I935"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14427,7 +14427,7 @@
         <v>31</v>
       </c>
       <c r="E466" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="F466">
         <v>90</v>
@@ -27554,6 +27554,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I935" xr:uid="{5DE63C91-ED9B-4686-95AA-68C8A03DF8A9}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K133" r:id="rId1" xr:uid="{FA683650-69E0-43B5-9F35-B73B24D0D61A}"/>

</xml_diff>

<commit_message>
fix bha sou game
</commit_message>
<xml_diff>
--- a/Data/EPL_fixtures.xlsx
+++ b/Data/EPL_fixtures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshua.mark\Downloads\EPL_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F389076-CDAA-42FD-A4C9-E326296E9B86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A09C90-BFF8-4D5E-9548-36E509D345E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FB97F535-5B47-48FC-ABD3-A15F766655E8}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="16170" xr2:uid="{FB97F535-5B47-48FC-ABD3-A15F766655E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Goals" sheetId="3" r:id="rId1"/>
@@ -3464,7 +3464,7 @@
         <v>26</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F73" s="3">
         <v>55</v>
@@ -3491,7 +3491,7 @@
         <v>26</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F74" s="3">
         <v>90</v>
@@ -3518,7 +3518,7 @@
         <v>26</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="F75" s="3">
         <v>90</v>

</xml_diff>